<commit_message>
Hopefully the last motor tests
</commit_message>
<xml_diff>
--- a/Test Results/Motor Ra (New tests).xlsb.xlsx
+++ b/Test Results/Motor Ra (New tests).xlsb.xlsx
@@ -486,6 +486,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,7 +517,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7442,7 +7442,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -7479,7 +7479,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -13889,8 +13889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:BK172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ14" sqref="AZ14"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BF5" sqref="BF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14020,7 +14020,7 @@
       <c r="AY10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AZ10" s="36">
+      <c r="AZ10" s="26">
         <v>1.4200000000000001E-4</v>
       </c>
     </row>
@@ -14351,76 +14351,76 @@
       <c r="AW25" s="17"/>
     </row>
     <row r="26" spans="1:59" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="AN26" s="26"/>
-      <c r="AO26" s="26"/>
-      <c r="AP26" s="26"/>
-      <c r="AQ26" s="26"/>
-      <c r="AR26" s="26"/>
-      <c r="AS26" s="26"/>
-      <c r="AT26" s="26"/>
-      <c r="AU26" s="26"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="27"/>
+      <c r="AP26" s="27"/>
+      <c r="AQ26" s="27"/>
+      <c r="AR26" s="27"/>
+      <c r="AS26" s="27"/>
+      <c r="AT26" s="27"/>
+      <c r="AU26" s="27"/>
       <c r="AW26" s="17"/>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.3">
       <c r="AW27" s="17"/>
     </row>
     <row r="28" spans="1:59" ht="21" x14ac:dyDescent="0.4">
-      <c r="K28" s="26" t="s">
+      <c r="K28" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
       <c r="R28" t="s">
         <v>24</v>
       </c>
-      <c r="AE28" s="26" t="s">
+      <c r="AE28" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="AF28" s="26"/>
-      <c r="AG28" s="26"/>
-      <c r="AH28" s="26"/>
-      <c r="AI28" s="26"/>
-      <c r="AJ28" s="26"/>
-      <c r="AK28" s="26"/>
-      <c r="AN28" s="26" t="s">
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="27"/>
+      <c r="AH28" s="27"/>
+      <c r="AI28" s="27"/>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+      <c r="AN28" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="AO28" s="26"/>
-      <c r="AP28" s="26"/>
-      <c r="AQ28" s="26"/>
-      <c r="AR28" s="26"/>
-      <c r="AS28" s="26"/>
-      <c r="AT28" s="26"/>
-      <c r="AU28" s="26"/>
+      <c r="AO28" s="27"/>
+      <c r="AP28" s="27"/>
+      <c r="AQ28" s="27"/>
+      <c r="AR28" s="27"/>
+      <c r="AS28" s="27"/>
+      <c r="AT28" s="27"/>
+      <c r="AU28" s="27"/>
       <c r="AW28" s="17"/>
-      <c r="AY28" s="26" t="s">
+      <c r="AY28" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="AZ28" s="26"/>
-      <c r="BA28" s="26"/>
-      <c r="BB28" s="26"/>
-      <c r="BC28" s="26"/>
-      <c r="BD28" s="26"/>
-      <c r="BE28" s="26"/>
+      <c r="AZ28" s="27"/>
+      <c r="BA28" s="27"/>
+      <c r="BB28" s="27"/>
+      <c r="BC28" s="27"/>
+      <c r="BD28" s="27"/>
+      <c r="BE28" s="27"/>
     </row>
     <row r="29" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AW29" s="17"/>
     </row>
     <row r="30" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H30" s="28" t="s">
+      <c r="H30" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="L30" s="31" t="s">
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="L30" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="32"/>
-      <c r="N30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="34"/>
       <c r="AN30" s="2" t="s">
         <v>57</v>
       </c>
@@ -16399,28 +16399,28 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="AW56" s="17"/>
-      <c r="AZ56" s="26" t="s">
+      <c r="AZ56" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="BA56" s="26"/>
-      <c r="BB56" s="26"/>
-      <c r="BC56" s="26"/>
-      <c r="BD56" s="26"/>
-      <c r="BE56" s="26"/>
-      <c r="BF56" s="26"/>
-      <c r="BG56" s="26"/>
+      <c r="BA56" s="27"/>
+      <c r="BB56" s="27"/>
+      <c r="BC56" s="27"/>
+      <c r="BD56" s="27"/>
+      <c r="BE56" s="27"/>
+      <c r="BF56" s="27"/>
+      <c r="BG56" s="27"/>
     </row>
     <row r="57" spans="4:62" ht="21" x14ac:dyDescent="0.4">
-      <c r="H57" s="26" t="s">
+      <c r="H57" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
-      <c r="N57" s="26"/>
-      <c r="O57" s="26"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
       <c r="AW57" s="17"/>
     </row>
     <row r="58" spans="4:62" x14ac:dyDescent="0.3">
@@ -16681,11 +16681,11 @@
         <v>9.3399999999999997E-2</v>
       </c>
       <c r="BH62" s="4">
-        <f>BG62/BF62</f>
+        <f t="shared" ref="BH62:BH77" si="25">BG62/BF62</f>
         <v>3.7359999999999997E-2</v>
       </c>
       <c r="BJ62" s="4">
-        <f t="shared" ref="BJ62:BJ64" si="25">AVERAGE(BC62,BH62)</f>
+        <f t="shared" ref="BJ62:BJ64" si="26">AVERAGE(BC62,BH62)</f>
         <v>3.304E-2</v>
       </c>
     </row>
@@ -16701,7 +16701,7 @@
         <v>1.54E-2</v>
       </c>
       <c r="H63" s="4">
-        <f t="shared" ref="H63:H69" si="26">G63/F63</f>
+        <f t="shared" ref="H63:H69" si="27">G63/F63</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="J63">
@@ -16744,11 +16744,11 @@
         <v>0.1134</v>
       </c>
       <c r="BH63" s="4">
-        <f>BG63/BF63</f>
+        <f t="shared" si="25"/>
         <v>3.78E-2</v>
       </c>
       <c r="BJ63" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -16764,7 +16764,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H64" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="J64">
@@ -16807,11 +16807,11 @@
         <v>0.12859999999999999</v>
       </c>
       <c r="BH64" s="4">
-        <f>BG64/BF64</f>
+        <f t="shared" si="25"/>
         <v>3.674285714285714E-2</v>
       </c>
       <c r="BJ64" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3.2885714285714282E-2</v>
       </c>
     </row>
@@ -16827,7 +16827,7 @@
         <v>1.9800000000000002E-2</v>
       </c>
       <c r="H65" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.6000000000000008E-3</v>
       </c>
       <c r="J65">
@@ -16870,11 +16870,11 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="BH65" s="4">
-        <f>BG65/BF65</f>
+        <f t="shared" si="25"/>
         <v>3.6249999999999998E-2</v>
       </c>
       <c r="BJ65" s="4">
-        <f>AVERAGE(BC65,BH65)</f>
+        <f t="shared" ref="BJ65:BJ77" si="28">AVERAGE(BC65,BH65)</f>
         <v>3.2674999999999996E-2</v>
       </c>
     </row>
@@ -16890,7 +16890,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="H66" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.2857142857142851E-3</v>
       </c>
       <c r="J66">
@@ -16939,11 +16939,11 @@
         <v>0.15959999999999999</v>
       </c>
       <c r="BH66" s="4">
-        <f>BG66/BF66</f>
+        <f t="shared" si="25"/>
         <v>3.5466666666666667E-2</v>
       </c>
       <c r="BJ66" s="4">
-        <f>AVERAGE(BC66,BH66)</f>
+        <f t="shared" si="28"/>
         <v>3.2333333333333332E-2</v>
       </c>
     </row>
@@ -16959,7 +16959,7 @@
         <v>2.58E-2</v>
       </c>
       <c r="H67" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.45E-3</v>
       </c>
       <c r="J67">
@@ -17011,11 +17011,11 @@
         <v>0.1744</v>
       </c>
       <c r="BH67" s="4">
-        <f>BG67/BF67</f>
+        <f t="shared" si="25"/>
         <v>3.4880000000000001E-2</v>
       </c>
       <c r="BJ67" s="4">
-        <f>AVERAGE(BC67,BH67)</f>
+        <f t="shared" si="28"/>
         <v>3.2419999999999997E-2</v>
       </c>
       <c r="BK67" s="4"/>
@@ -17032,7 +17032,7 @@
         <v>3.04E-2</v>
       </c>
       <c r="H68" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.7555555555555554E-3</v>
       </c>
       <c r="J68">
@@ -17050,7 +17050,7 @@
         <v>7.244444444444444E-3</v>
       </c>
       <c r="O68" s="4">
-        <f t="shared" ref="O68:O80" si="27">AVERAGE(H68,M68)</f>
+        <f t="shared" ref="O68:O80" si="29">AVERAGE(H68,M68)</f>
         <v>6.9999999999999993E-3</v>
       </c>
       <c r="P68" s="4">
@@ -17084,11 +17084,11 @@
         <v>0.185</v>
       </c>
       <c r="BH68" s="4">
-        <f>BG68/BF68</f>
+        <f t="shared" si="25"/>
         <v>3.3636363636363638E-2</v>
       </c>
       <c r="BJ68" s="4">
-        <f>AVERAGE(BC68,BH68)</f>
+        <f t="shared" si="28"/>
         <v>3.1418181818181817E-2</v>
       </c>
       <c r="BK68" s="4"/>
@@ -17105,7 +17105,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
       <c r="H69" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>6.5600000000000007E-3</v>
       </c>
       <c r="J69">
@@ -17123,7 +17123,7 @@
         <v>7.0800000000000004E-3</v>
       </c>
       <c r="O69" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.8200000000000005E-3</v>
       </c>
       <c r="P69" s="4">
@@ -17157,11 +17157,11 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="BH69" s="4">
-        <f>BG69/BF69</f>
+        <f t="shared" si="25"/>
         <v>3.266666666666667E-2</v>
       </c>
       <c r="BJ69" s="4">
-        <f>AVERAGE(BC69,BH69)</f>
+        <f t="shared" si="28"/>
         <v>3.1533333333333337E-2</v>
       </c>
       <c r="BK69" s="4"/>
@@ -17174,11 +17174,11 @@
         <v>5.5</v>
       </c>
       <c r="G70">
-        <f t="shared" ref="G70:G80" si="28">E70/(5*1000)</f>
+        <f t="shared" ref="G70:G80" si="30">E70/(5*1000)</f>
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="H70" s="4">
-        <f t="shared" ref="H70:H80" si="29">G70/F70</f>
+        <f t="shared" ref="H70:H80" si="31">G70/F70</f>
         <v>6.1090909090909086E-3</v>
       </c>
       <c r="J70">
@@ -17196,11 +17196,11 @@
         <v>6.909090909090909E-3</v>
       </c>
       <c r="O70" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.5090909090909088E-3</v>
       </c>
       <c r="P70" s="4">
-        <f t="shared" ref="P70:P80" si="30">0.0064*F70</f>
+        <f t="shared" ref="P70:P80" si="32">0.0064*F70</f>
         <v>3.5200000000000002E-2</v>
       </c>
       <c r="Q70" s="4"/>
@@ -17230,11 +17230,11 @@
         <v>0.21479999999999999</v>
       </c>
       <c r="BH70" s="4">
-        <f>BG70/BF70</f>
+        <f t="shared" si="25"/>
         <v>3.3046153846153843E-2</v>
       </c>
       <c r="BJ70" s="4">
-        <f>AVERAGE(BC70,BH70)</f>
+        <f t="shared" si="28"/>
         <v>3.1107692307692305E-2</v>
       </c>
       <c r="BK70" s="4"/>
@@ -17247,11 +17247,11 @@
         <v>6</v>
       </c>
       <c r="G71">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>3.6200000000000003E-2</v>
       </c>
       <c r="H71" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.0333333333333341E-3</v>
       </c>
       <c r="J71">
@@ -17269,11 +17269,11 @@
         <v>6.8333333333333336E-3</v>
       </c>
       <c r="O71" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.4333333333333343E-3</v>
       </c>
       <c r="P71" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>3.8400000000000004E-2</v>
       </c>
       <c r="Q71" s="4"/>
@@ -17303,11 +17303,11 @@
         <v>0.22439999999999999</v>
       </c>
       <c r="BH71" s="4">
-        <f>BG71/BF71</f>
+        <f t="shared" si="25"/>
         <v>3.2057142857142853E-2</v>
       </c>
       <c r="BJ71" s="4">
-        <f>AVERAGE(BC71,BH71)</f>
+        <f t="shared" si="28"/>
         <v>3.0671428571428568E-2</v>
       </c>
       <c r="BK71" s="4"/>
@@ -17320,11 +17320,11 @@
         <v>6.5</v>
       </c>
       <c r="G72">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.1399999999999999E-2</v>
       </c>
       <c r="H72" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.3692307692307694E-3</v>
       </c>
       <c r="J72">
@@ -17342,11 +17342,11 @@
         <v>6.7384615384615387E-3</v>
       </c>
       <c r="O72" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.553846153846154E-3</v>
       </c>
       <c r="P72" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>4.1600000000000005E-2</v>
       </c>
       <c r="Q72" s="4"/>
@@ -17376,11 +17376,11 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="BH72" s="4">
-        <f>BG72/BF72</f>
+        <f t="shared" si="25"/>
         <v>3.1733333333333329E-2</v>
       </c>
       <c r="BJ72" s="4">
-        <f>AVERAGE(BC72,BH72)</f>
+        <f t="shared" si="28"/>
         <v>3.048E-2</v>
       </c>
       <c r="BK72" s="4"/>
@@ -17393,11 +17393,11 @@
         <v>7</v>
       </c>
       <c r="G73">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.3200000000000002E-2</v>
       </c>
       <c r="H73" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.1714285714285716E-3</v>
       </c>
       <c r="J73">
@@ -17415,11 +17415,11 @@
         <v>6.6857142857142862E-3</v>
       </c>
       <c r="O73" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.4285714285714293E-3</v>
       </c>
       <c r="P73" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>4.48E-2</v>
       </c>
       <c r="Q73" s="4"/>
@@ -17449,11 +17449,11 @@
         <v>0.25259999999999999</v>
       </c>
       <c r="BH73" s="4">
-        <f>BG73/BF73</f>
+        <f t="shared" si="25"/>
         <v>3.1574999999999999E-2</v>
       </c>
       <c r="BJ73" s="4">
-        <f>AVERAGE(BC73,BH73)</f>
+        <f t="shared" si="28"/>
         <v>3.0362500000000001E-2</v>
       </c>
       <c r="BK73" s="4"/>
@@ -17466,11 +17466,11 @@
         <v>7.5</v>
       </c>
       <c r="G74">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.48E-2</v>
       </c>
       <c r="H74" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>5.9733333333333331E-3</v>
       </c>
       <c r="J74">
@@ -17488,11 +17488,11 @@
         <v>6.613333333333333E-3</v>
       </c>
       <c r="O74" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2933333333333331E-3</v>
       </c>
       <c r="P74" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="Q74" s="4"/>
@@ -17522,11 +17522,11 @@
         <v>0.26579999999999998</v>
       </c>
       <c r="BH74" s="4">
-        <f>BG74/BF74</f>
+        <f t="shared" si="25"/>
         <v>3.1270588235294113E-2</v>
       </c>
       <c r="BJ74" s="4">
-        <f>AVERAGE(BC74,BH74)</f>
+        <f t="shared" si="28"/>
         <v>3.0211764705882348E-2</v>
       </c>
       <c r="BK74" s="4"/>
@@ -17539,11 +17539,11 @@
         <v>8</v>
       </c>
       <c r="G75">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.8399999999999999E-2</v>
       </c>
       <c r="H75" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.0499999999999998E-3</v>
       </c>
       <c r="J75">
@@ -17561,11 +17561,11 @@
         <v>6.45E-3</v>
       </c>
       <c r="O75" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="P75" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>5.1200000000000002E-2</v>
       </c>
       <c r="Q75" s="4"/>
@@ -17595,11 +17595,11 @@
         <v>0.2802</v>
       </c>
       <c r="BH75" s="4">
-        <f>BG75/BF75</f>
+        <f t="shared" si="25"/>
         <v>3.1133333333333332E-2</v>
       </c>
       <c r="BJ75" s="4">
-        <f>AVERAGE(BC75,BH75)</f>
+        <f t="shared" si="28"/>
         <v>3.0033333333333335E-2</v>
       </c>
       <c r="BK75" s="4"/>
@@ -17612,11 +17612,11 @@
         <v>8.5</v>
       </c>
       <c r="G76">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>5.2400000000000002E-2</v>
       </c>
       <c r="H76" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.1647058823529411E-3</v>
       </c>
       <c r="J76">
@@ -17634,11 +17634,11 @@
         <v>6.3764705882352942E-3</v>
       </c>
       <c r="O76" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2705882352941181E-3</v>
       </c>
       <c r="P76" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>5.4400000000000004E-2</v>
       </c>
       <c r="Q76" s="4"/>
@@ -17668,11 +17668,11 @@
         <v>0.29139999999999999</v>
       </c>
       <c r="BH76" s="4">
-        <f>BG76/BF76</f>
+        <f t="shared" si="25"/>
         <v>3.0673684210526315E-2</v>
       </c>
       <c r="BJ76" s="4">
-        <f>AVERAGE(BC76,BH76)</f>
+        <f t="shared" si="28"/>
         <v>2.9810526315789475E-2</v>
       </c>
       <c r="BK76" s="4"/>
@@ -17685,11 +17685,11 @@
         <v>9</v>
       </c>
       <c r="G77">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>5.5399999999999998E-2</v>
       </c>
       <c r="H77" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.1555555555555556E-3</v>
       </c>
       <c r="J77">
@@ -17707,11 +17707,11 @@
         <v>6.3111111111111111E-3</v>
       </c>
       <c r="O77" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2333333333333338E-3</v>
       </c>
       <c r="P77" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>5.7600000000000005E-2</v>
       </c>
       <c r="Q77" s="4"/>
@@ -17741,11 +17741,11 @@
         <v>0.29620000000000002</v>
       </c>
       <c r="BH77" s="4">
-        <f>BG77/BF77</f>
+        <f t="shared" si="25"/>
         <v>2.962E-2</v>
       </c>
       <c r="BJ77" s="4">
-        <f>AVERAGE(BC77,BH77)</f>
+        <f t="shared" si="28"/>
         <v>2.9309999999999999E-2</v>
       </c>
       <c r="BK77" s="4"/>
@@ -17758,11 +17758,11 @@
         <v>9.5</v>
       </c>
       <c r="G78">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>5.6599999999999998E-2</v>
       </c>
       <c r="H78" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>5.9578947368421047E-3</v>
       </c>
       <c r="J78">
@@ -17780,19 +17780,19 @@
         <v>6.1052631578947369E-3</v>
       </c>
       <c r="O78" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.0315789473684208E-3</v>
       </c>
       <c r="P78" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>6.08E-2</v>
       </c>
       <c r="Q78" s="4"/>
       <c r="AW78" s="17"/>
-      <c r="BA78" s="34" t="s">
+      <c r="BA78" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="BB78" s="35"/>
+      <c r="BB78" s="36"/>
       <c r="BC78" s="6">
         <f>AVERAGE(BC65:BC77)</f>
         <v>2.9286558050189863E-2</v>
@@ -17818,11 +17818,11 @@
         <v>10</v>
       </c>
       <c r="G79">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>6.1800000000000001E-2</v>
       </c>
       <c r="H79" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.1799999999999997E-3</v>
       </c>
       <c r="J79">
@@ -17840,11 +17840,11 @@
         <v>6.1799999999999997E-3</v>
       </c>
       <c r="O79" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.1799999999999997E-3</v>
       </c>
       <c r="P79" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="Q79" s="4"/>
@@ -17859,11 +17859,11 @@
         <v>10.37</v>
       </c>
       <c r="G80">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>6.2799999999999995E-2</v>
       </c>
       <c r="H80" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.0559305689488908E-3</v>
       </c>
       <c r="J80">
@@ -17881,11 +17881,11 @@
         <v>6.0559305689488908E-3</v>
       </c>
       <c r="O80" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.0559305689488908E-3</v>
       </c>
       <c r="P80" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>6.6367999999999996E-2</v>
       </c>
       <c r="Q80" s="4"/>
@@ -17904,15 +17904,15 @@
     </row>
     <row r="82" spans="4:63" ht="21" x14ac:dyDescent="0.4">
       <c r="AW82" s="17"/>
-      <c r="BB82" s="26" t="s">
+      <c r="BB82" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="BC82" s="26"/>
-      <c r="BD82" s="26"/>
-      <c r="BE82" s="26"/>
-      <c r="BF82" s="26"/>
-      <c r="BG82" s="26"/>
-      <c r="BH82" s="26"/>
+      <c r="BC82" s="27"/>
+      <c r="BD82" s="27"/>
+      <c r="BE82" s="27"/>
+      <c r="BF82" s="27"/>
+      <c r="BG82" s="27"/>
+      <c r="BH82" s="27"/>
     </row>
     <row r="83" spans="4:63" ht="21" x14ac:dyDescent="0.4">
       <c r="AW83" s="17"/>
@@ -17930,15 +17930,15 @@
       <c r="AW84" s="17"/>
     </row>
     <row r="85" spans="4:63" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I85" s="26" t="s">
+      <c r="I85" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="J85" s="26"/>
-      <c r="K85" s="26"/>
-      <c r="L85" s="26"/>
-      <c r="M85" s="26"/>
-      <c r="N85" s="26"/>
-      <c r="O85" s="26"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="27"/>
+      <c r="M85" s="27"/>
+      <c r="N85" s="27"/>
+      <c r="O85" s="27"/>
       <c r="AW85" s="17"/>
       <c r="BC85" s="15"/>
       <c r="BD85" s="2" t="s">
@@ -17985,15 +17985,15 @@
         <v>850</v>
       </c>
       <c r="BF86">
-        <f t="shared" ref="BF86:BF87" si="31">BE86</f>
+        <f t="shared" ref="BF86:BF87" si="33">BE86</f>
         <v>850</v>
       </c>
       <c r="BG86">
-        <f t="shared" ref="BG86:BG100" si="32">BF86*2*PI()/60</f>
+        <f t="shared" ref="BG86:BG100" si="34">BF86*2*PI()/60</f>
         <v>89.011791851710797</v>
       </c>
       <c r="BI86">
-        <f>$BA$87*BD86/BG86</f>
+        <f t="shared" ref="BI86:BI98" si="35">$BA$87*BD86/BG86</f>
         <v>2.4347395447611096E-4</v>
       </c>
     </row>
@@ -18032,15 +18032,15 @@
         <v>925</v>
       </c>
       <c r="BF87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>925</v>
       </c>
       <c r="BG87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>96.865773485685295</v>
       </c>
       <c r="BI87">
-        <f>$BA$87*BD87/BG87</f>
+        <f t="shared" si="35"/>
         <v>2.297796560870236E-4</v>
       </c>
     </row>
@@ -18081,15 +18081,15 @@
         <v>1020</v>
       </c>
       <c r="BG88">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>106.81415022205297</v>
       </c>
       <c r="BI88">
-        <f>$BA$87*BD88/BG88</f>
+        <f t="shared" si="35"/>
         <v>2.1386225731009746E-4</v>
       </c>
       <c r="BJ88">
-        <f>BI88*BG88</f>
+        <f t="shared" ref="BJ88:BJ98" si="36">BI88*BG88</f>
         <v>2.2843515279148095E-2</v>
       </c>
     </row>
@@ -18104,11 +18104,11 @@
         <v>6</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89:H96" si="33">0.33*G89</f>
+        <f t="shared" ref="H89:H96" si="37">0.33*G89</f>
         <v>1.98</v>
       </c>
       <c r="I89">
-        <f t="shared" ref="I89:I96" si="34">H89/F89</f>
+        <f t="shared" ref="I89:I96" si="38">H89/F89</f>
         <v>0.99</v>
       </c>
       <c r="J89">
@@ -18124,19 +18124,19 @@
         <v>111</v>
       </c>
       <c r="BF89">
-        <f t="shared" ref="BF89:BF100" si="35">BE89/0.1</f>
+        <f t="shared" ref="BF89:BF100" si="39">BE89/0.1</f>
         <v>1110</v>
       </c>
       <c r="BG89">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>116.23892818282235</v>
       </c>
       <c r="BI89">
-        <f>$BA$87*BD89/BG89</f>
+        <f t="shared" si="35"/>
         <v>2.0156110183072246E-4</v>
       </c>
       <c r="BJ89">
-        <f>BI89*BG89</f>
+        <f t="shared" si="36"/>
         <v>2.3429246440151891E-2</v>
       </c>
     </row>
@@ -18151,11 +18151,11 @@
         <v>7.4</v>
       </c>
       <c r="H90">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.4420000000000002</v>
       </c>
       <c r="I90">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.97680000000000011</v>
       </c>
       <c r="J90">
@@ -18173,19 +18173,19 @@
         <v>123</v>
       </c>
       <c r="BF90">
+        <f t="shared" si="39"/>
+        <v>1230</v>
+      </c>
+      <c r="BG90">
+        <f t="shared" si="34"/>
+        <v>128.80529879718151</v>
+      </c>
+      <c r="BI90">
         <f t="shared" si="35"/>
-        <v>1230</v>
-      </c>
-      <c r="BG90">
-        <f t="shared" si="32"/>
-        <v>128.80529879718151</v>
-      </c>
-      <c r="BI90">
-        <f>$BA$87*BD90/BG90</f>
         <v>1.864440191934183E-4</v>
       </c>
       <c r="BJ90">
-        <f>BI90*BG90</f>
+        <f t="shared" si="36"/>
         <v>2.4014977601155688E-2</v>
       </c>
     </row>
@@ -18200,11 +18200,11 @@
         <v>8.9</v>
       </c>
       <c r="H91">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.9370000000000003</v>
       </c>
       <c r="I91">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.97900000000000009</v>
       </c>
       <c r="J91">
@@ -18220,19 +18220,19 @@
         <v>138</v>
       </c>
       <c r="BF91">
+        <f t="shared" si="39"/>
+        <v>1380</v>
+      </c>
+      <c r="BG91">
+        <f t="shared" si="34"/>
+        <v>144.5132620651305</v>
+      </c>
+      <c r="BI91">
         <f t="shared" si="35"/>
-        <v>1380</v>
-      </c>
-      <c r="BG91">
-        <f t="shared" si="32"/>
-        <v>144.5132620651305</v>
-      </c>
-      <c r="BI91">
-        <f>$BA$87*BD91/BG91</f>
         <v>1.7023149578529492E-4</v>
       </c>
       <c r="BJ91">
-        <f>BI91*BG91</f>
+        <f t="shared" si="36"/>
         <v>2.4600708762159484E-2</v>
       </c>
     </row>
@@ -18247,11 +18247,11 @@
         <v>10.3</v>
       </c>
       <c r="H92">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3.3990000000000005</v>
       </c>
       <c r="I92">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.97114285714285731</v>
       </c>
       <c r="J92">
@@ -18267,19 +18267,19 @@
         <v>144</v>
       </c>
       <c r="BF92">
+        <f t="shared" si="39"/>
+        <v>1440</v>
+      </c>
+      <c r="BG92">
+        <f t="shared" si="34"/>
+        <v>150.79644737231007</v>
+      </c>
+      <c r="BI92">
         <f t="shared" si="35"/>
-        <v>1440</v>
-      </c>
-      <c r="BG92">
-        <f t="shared" si="32"/>
-        <v>150.79644737231007</v>
-      </c>
-      <c r="BI92">
-        <f>$BA$87*BD92/BG92</f>
         <v>1.6702276719410389E-4</v>
       </c>
       <c r="BJ92">
-        <f>BI92*BG92</f>
+        <f t="shared" si="36"/>
         <v>2.5186439923163283E-2</v>
       </c>
     </row>
@@ -18294,11 +18294,11 @@
         <v>15.3</v>
       </c>
       <c r="H93">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>5.0490000000000004</v>
       </c>
       <c r="I93">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1.2622500000000001</v>
       </c>
       <c r="J93">
@@ -18314,19 +18314,19 @@
         <v>158</v>
       </c>
       <c r="BF93">
+        <f t="shared" si="39"/>
+        <v>1580</v>
+      </c>
+      <c r="BG93">
+        <f t="shared" si="34"/>
+        <v>165.45721308906244</v>
+      </c>
+      <c r="BI93">
         <f t="shared" si="35"/>
-        <v>1580</v>
-      </c>
-      <c r="BG93">
-        <f t="shared" si="32"/>
-        <v>165.45721308906244</v>
-      </c>
-      <c r="BI93">
-        <f>$BA$87*BD93/BG93</f>
         <v>1.5576335780715959E-4</v>
       </c>
       <c r="BJ93">
-        <f>BI93*BG93</f>
+        <f t="shared" si="36"/>
         <v>2.577217108416708E-2</v>
       </c>
     </row>
@@ -18341,11 +18341,11 @@
         <v>16.399999999999999</v>
       </c>
       <c r="H94">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>5.4119999999999999</v>
       </c>
       <c r="I94">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1.2026666666666666</v>
       </c>
       <c r="J94">
@@ -18361,19 +18361,19 @@
         <v>176</v>
       </c>
       <c r="BF94">
+        <f t="shared" si="39"/>
+        <v>1760</v>
+      </c>
+      <c r="BG94">
+        <f t="shared" si="34"/>
+        <v>184.30676901060122</v>
+      </c>
+      <c r="BI94">
         <f t="shared" si="35"/>
-        <v>1760</v>
-      </c>
-      <c r="BG94">
-        <f t="shared" si="32"/>
-        <v>184.30676901060122</v>
-      </c>
-      <c r="BI94">
-        <f>$BA$87*BD94/BG94</f>
         <v>1.4301103744949697E-4</v>
       </c>
       <c r="BJ94">
-        <f>BI94*BG94</f>
+        <f t="shared" si="36"/>
         <v>2.6357902245170879E-2</v>
       </c>
     </row>
@@ -18388,11 +18388,11 @@
         <v>18.8</v>
       </c>
       <c r="H95">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>6.2040000000000006</v>
       </c>
       <c r="I95">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1.2408000000000001</v>
       </c>
       <c r="J95">
@@ -18408,19 +18408,19 @@
         <v>195</v>
       </c>
       <c r="BF95">
+        <f t="shared" si="39"/>
+        <v>1950</v>
+      </c>
+      <c r="BG95">
+        <f t="shared" si="34"/>
+        <v>204.20352248333657</v>
+      </c>
+      <c r="BI95">
         <f t="shared" si="35"/>
-        <v>1950</v>
-      </c>
-      <c r="BG95">
-        <f t="shared" si="32"/>
-        <v>204.20352248333657</v>
-      </c>
-      <c r="BI95">
-        <f>$BA$87*BD95/BG95</f>
         <v>1.319449981984191E-4</v>
       </c>
       <c r="BJ95">
-        <f>BI95*BG95</f>
+        <f t="shared" si="36"/>
         <v>2.6943633406174679E-2</v>
       </c>
     </row>
@@ -18435,11 +18435,11 @@
         <v>22.2</v>
       </c>
       <c r="H96">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>7.3260000000000005</v>
       </c>
       <c r="I96">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1.3320000000000001</v>
       </c>
       <c r="J96">
@@ -18455,19 +18455,19 @@
         <v>207</v>
       </c>
       <c r="BF96">
+        <f t="shared" si="39"/>
+        <v>2070</v>
+      </c>
+      <c r="BG96">
+        <f t="shared" si="34"/>
+        <v>216.76989309769573</v>
+      </c>
+      <c r="BI96">
         <f t="shared" si="35"/>
-        <v>2070</v>
-      </c>
-      <c r="BG96">
-        <f t="shared" si="32"/>
-        <v>216.76989309769573</v>
-      </c>
-      <c r="BI96">
-        <f>$BA$87*BD96/BG96</f>
         <v>1.2699810003029941E-4</v>
       </c>
       <c r="BJ96">
-        <f>BI96*BG96</f>
+        <f t="shared" si="36"/>
         <v>2.7529364567178471E-2</v>
       </c>
     </row>
@@ -18484,19 +18484,19 @@
         <v>222</v>
       </c>
       <c r="BF97">
+        <f t="shared" si="39"/>
+        <v>2220</v>
+      </c>
+      <c r="BG97">
+        <f t="shared" si="34"/>
+        <v>232.4778563656447</v>
+      </c>
+      <c r="BI97">
         <f t="shared" si="35"/>
-        <v>2220</v>
-      </c>
-      <c r="BG97">
-        <f t="shared" si="32"/>
-        <v>232.4778563656447</v>
-      </c>
-      <c r="BI97">
-        <f>$BA$87*BD97/BG97</f>
         <v>1.2093666109843348E-4</v>
       </c>
       <c r="BJ97">
-        <f>BI97*BG97</f>
+        <f t="shared" si="36"/>
         <v>2.8115095728182268E-2</v>
       </c>
     </row>
@@ -18520,19 +18520,19 @@
         <v>241</v>
       </c>
       <c r="BF98">
+        <f t="shared" si="39"/>
+        <v>2410</v>
+      </c>
+      <c r="BG98">
+        <f t="shared" si="34"/>
+        <v>252.37460983838002</v>
+      </c>
+      <c r="BI98">
         <f t="shared" si="35"/>
-        <v>2410</v>
-      </c>
-      <c r="BG98">
-        <f t="shared" si="32"/>
-        <v>252.37460983838002</v>
-      </c>
-      <c r="BI98">
-        <f>$BA$87*BD98/BG98</f>
         <v>1.137231154416286E-4</v>
       </c>
       <c r="BJ98">
-        <f>BI98*BG98</f>
+        <f t="shared" si="36"/>
         <v>2.8700826889186067E-2</v>
       </c>
     </row>
@@ -18549,19 +18549,19 @@
         <v>276</v>
       </c>
       <c r="BF99">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>2760</v>
       </c>
       <c r="BG99">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>289.02652413026101</v>
       </c>
       <c r="BI99">
-        <f t="shared" ref="BI99:BI100" si="36">$BA$87*BD99/BG99</f>
+        <f t="shared" ref="BI99:BI100" si="40">$BA$87*BD99/BG99</f>
         <v>1.0132827130077079E-4</v>
       </c>
       <c r="BJ99">
-        <f t="shared" ref="BJ99:BJ100" si="37">BI99*BG99</f>
+        <f t="shared" ref="BJ99:BJ100" si="41">BI99*BG99</f>
         <v>2.9286558050189863E-2</v>
       </c>
     </row>
@@ -18582,29 +18582,29 @@
         <v>307</v>
       </c>
       <c r="BF100">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>3070</v>
       </c>
       <c r="BG100">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>321.48964821735547</v>
       </c>
       <c r="BI100">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>9.3829319105482502E-5</v>
       </c>
       <c r="BJ100">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>3.0165154791695559E-2</v>
       </c>
     </row>
     <row r="101" spans="3:62" x14ac:dyDescent="0.3">
-      <c r="G101" s="27" t="s">
+      <c r="G101" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
       <c r="AW101" s="17"/>
       <c r="BC101" s="19"/>
     </row>
@@ -18668,11 +18668,11 @@
         <v>5.4250000000000007</v>
       </c>
       <c r="H104">
-        <f t="shared" ref="H104:H116" si="38">0.33*G104</f>
+        <f t="shared" ref="H104:H116" si="42">0.33*G104</f>
         <v>1.7902500000000003</v>
       </c>
       <c r="I104">
-        <f t="shared" ref="I104:I113" si="39">H104/F104</f>
+        <f t="shared" ref="I104:I113" si="43">H104/F104</f>
         <v>0.89512500000000017</v>
       </c>
       <c r="J104">
@@ -18690,11 +18690,11 @@
         <v>7.4250000000000007</v>
       </c>
       <c r="H105">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>2.4502500000000005</v>
       </c>
       <c r="I105">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0.98010000000000019</v>
       </c>
       <c r="J105">
@@ -18712,11 +18712,11 @@
         <v>8.9250000000000007</v>
       </c>
       <c r="H106">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>2.9452500000000006</v>
       </c>
       <c r="I106">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0.98175000000000023</v>
       </c>
       <c r="J106">
@@ -18734,11 +18734,11 @@
         <v>10.925000000000001</v>
       </c>
       <c r="H107">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>3.6052500000000003</v>
       </c>
       <c r="I107">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.0300714285714287</v>
       </c>
       <c r="J107">
@@ -18756,11 +18756,11 @@
         <v>12.425000000000001</v>
       </c>
       <c r="H108">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>4.1002500000000008</v>
       </c>
       <c r="I108">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.0250625000000002</v>
       </c>
       <c r="J108">
@@ -18778,11 +18778,11 @@
         <v>14.425000000000001</v>
       </c>
       <c r="H109">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>4.7602500000000001</v>
       </c>
       <c r="I109">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.0578333333333334</v>
       </c>
       <c r="J109">
@@ -18800,11 +18800,11 @@
         <v>15.925000000000001</v>
       </c>
       <c r="H110">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>5.2552500000000002</v>
       </c>
       <c r="I110">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.05105</v>
       </c>
       <c r="J110">
@@ -18822,11 +18822,11 @@
         <v>17.425000000000001</v>
       </c>
       <c r="H111">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>5.7502500000000003</v>
       </c>
       <c r="I111">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.0455000000000001</v>
       </c>
       <c r="J111">
@@ -18844,11 +18844,11 @@
         <v>18.925000000000001</v>
       </c>
       <c r="H112">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>6.2452500000000004</v>
       </c>
       <c r="I112">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.040875</v>
       </c>
       <c r="J112">
@@ -18866,11 +18866,11 @@
         <v>20.925000000000001</v>
       </c>
       <c r="H113">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>6.9052500000000006</v>
       </c>
       <c r="I113">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>1.0623461538461538</v>
       </c>
       <c r="J113">
@@ -18888,7 +18888,7 @@
         <v>22.425000000000001</v>
       </c>
       <c r="H114">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>7.4002500000000007</v>
       </c>
       <c r="I114">
@@ -18910,7 +18910,7 @@
         <v>24.425000000000001</v>
       </c>
       <c r="H115">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>8.0602499999999999</v>
       </c>
       <c r="I115">
@@ -18932,7 +18932,7 @@
         <v>27.425000000000001</v>
       </c>
       <c r="H116">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>9.0502500000000001</v>
       </c>
       <c r="I116">
@@ -18980,15 +18980,15 @@
       <c r="AW125" s="17"/>
     </row>
     <row r="126" spans="4:49" ht="21" x14ac:dyDescent="0.4">
-      <c r="I126" s="26" t="s">
+      <c r="I126" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J126" s="26"/>
-      <c r="K126" s="26"/>
-      <c r="L126" s="26"/>
-      <c r="M126" s="26"/>
-      <c r="N126" s="26"/>
-      <c r="O126" s="26"/>
+      <c r="J126" s="27"/>
+      <c r="K126" s="27"/>
+      <c r="L126" s="27"/>
+      <c r="M126" s="27"/>
+      <c r="N126" s="27"/>
+      <c r="O126" s="27"/>
       <c r="AW126" s="17"/>
     </row>
     <row r="127" spans="4:49" x14ac:dyDescent="0.3">
@@ -19037,11 +19037,11 @@
         <v>215</v>
       </c>
       <c r="J129">
-        <f t="shared" ref="J129:J135" si="40">I129</f>
+        <f t="shared" ref="J129:J135" si="44">I129</f>
         <v>215</v>
       </c>
       <c r="K129">
-        <f t="shared" ref="K129:K146" si="41">J129*2*PI()/60</f>
+        <f t="shared" ref="K129:K146" si="45">J129*2*PI()/60</f>
         <v>22.51474735072685</v>
       </c>
       <c r="M129">
@@ -19068,15 +19068,15 @@
         <v>325</v>
       </c>
       <c r="J130">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>325</v>
       </c>
       <c r="K130">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>34.033920413889426</v>
       </c>
       <c r="M130">
-        <f t="shared" ref="M130:M146" si="42">$E$132/K130*((H130-$E$131*K130)/$E$130)</f>
+        <f t="shared" ref="M130:M146" si="46">$E$132/K130*((H130-$E$131*K130)/$E$130)</f>
         <v>1.6125579522699003E-2</v>
       </c>
       <c r="AW130" s="17"/>
@@ -19096,15 +19096,15 @@
         <v>420</v>
       </c>
       <c r="J131">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>420</v>
       </c>
       <c r="K131">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>43.982297150257104</v>
       </c>
       <c r="M131">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>1.3732466580216781E-2</v>
       </c>
       <c r="AW131" s="17"/>
@@ -19124,15 +19124,15 @@
         <v>555</v>
       </c>
       <c r="J132">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>555</v>
       </c>
       <c r="K132">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>58.119464091411174</v>
       </c>
       <c r="M132">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>1.117133763121049E-2</v>
       </c>
       <c r="AW132" s="17"/>
@@ -19147,19 +19147,19 @@
         <v>675</v>
       </c>
       <c r="J133">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>675</v>
       </c>
       <c r="K133">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>70.685834705770347</v>
       </c>
       <c r="M133">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>9.8784238976240869E-3</v>
       </c>
       <c r="N133">
-        <f t="shared" ref="N133:N146" si="43">M133*K133</f>
+        <f t="shared" ref="N133:N146" si="47">M133*K133</f>
         <v>0.69826463878098788</v>
       </c>
       <c r="AW133" s="17"/>
@@ -19173,19 +19173,19 @@
         <v>805</v>
       </c>
       <c r="J134">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>805</v>
       </c>
       <c r="K134">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>84.299402871326109</v>
       </c>
       <c r="M134">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>8.8350165554967938E-3</v>
       </c>
       <c r="N134">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.74478661998666007</v>
       </c>
       <c r="AW134" s="17"/>
@@ -19199,19 +19199,19 @@
         <v>930</v>
       </c>
       <c r="J135">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>930</v>
       </c>
       <c r="K135">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>97.389372261283583</v>
       </c>
       <c r="M135">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>8.1378884925822244E-3</v>
       </c>
       <c r="N135">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.79254385182490616</v>
       </c>
       <c r="AW135" s="17"/>
@@ -19231,15 +19231,15 @@
         <v>1225</v>
       </c>
       <c r="K136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>128.28170002158322</v>
       </c>
       <c r="M136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>6.2230432089794658E-3</v>
       </c>
       <c r="N136">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.79830256215565443</v>
       </c>
       <c r="AW136" s="17"/>
@@ -19253,19 +19253,19 @@
         <v>138.5</v>
       </c>
       <c r="J137">
-        <f t="shared" ref="J137:J146" si="44">I137/0.1</f>
+        <f t="shared" ref="J137:J146" si="48">I137/0.1</f>
         <v>1385</v>
       </c>
       <c r="K137">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>145.03686084072879</v>
       </c>
       <c r="M137">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>5.7737945699575322E-3</v>
       </c>
       <c r="N137">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.83741303956588609</v>
       </c>
       <c r="AW137" s="17"/>
@@ -19279,19 +19279,19 @@
         <v>153</v>
       </c>
       <c r="J138">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>1530</v>
       </c>
       <c r="K138">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>160.22122533307945</v>
       </c>
       <c r="M138">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>5.4938368311935838E-3</v>
       </c>
       <c r="N138">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.88022926887383834</v>
       </c>
       <c r="AW138" s="17"/>
@@ -19305,19 +19305,19 @@
         <v>169</v>
       </c>
       <c r="J139">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>1690</v>
       </c>
       <c r="K139">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>176.97638615222502</v>
       </c>
       <c r="M139">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>5.1947028994778228E-3</v>
       </c>
       <c r="N139">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.91933974628407011</v>
       </c>
       <c r="AW139" s="17"/>
@@ -19331,19 +19331,19 @@
         <v>179</v>
       </c>
       <c r="J140">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>1790</v>
       </c>
       <c r="K140">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>187.448361664191</v>
       </c>
       <c r="M140">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>5.1922205275326842E-3</v>
       </c>
       <c r="N140">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.97327323128518317</v>
       </c>
       <c r="AW140" s="17"/>
@@ -19357,19 +19357,19 @@
         <v>191</v>
       </c>
       <c r="J141">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>1910</v>
       </c>
       <c r="K141">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>200.01473227855016</v>
       </c>
       <c r="M141">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>5.1109520889308594E-3</v>
       </c>
       <c r="N141">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.0222657137560025</v>
       </c>
       <c r="AW141" s="17"/>
@@ -19383,19 +19383,19 @@
         <v>208</v>
       </c>
       <c r="J142">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>2080</v>
       </c>
       <c r="K142">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>217.8170906488923</v>
       </c>
       <c r="M142">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>4.8614444658430312E-3</v>
       </c>
       <c r="N142">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.0589056899010874</v>
       </c>
       <c r="AW142" s="17"/>
@@ -19409,19 +19409,19 @@
         <v>225</v>
       </c>
       <c r="J143">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>2250</v>
       </c>
       <c r="K143">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>235.61944901923451</v>
       </c>
       <c r="M143">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>4.6496402169106952E-3</v>
       </c>
       <c r="N143">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.095545666046172</v>
       </c>
       <c r="AW143" s="17"/>
@@ -19435,19 +19435,19 @@
         <v>240</v>
       </c>
       <c r="J144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>2400</v>
       </c>
       <c r="K144">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>251.32741228718345</v>
       </c>
       <c r="M144">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>4.524483160723407E-3</v>
       </c>
       <c r="N144">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.1371266447215507</v>
       </c>
       <c r="AW144" s="17"/>
@@ -19461,19 +19461,19 @@
         <v>253</v>
       </c>
       <c r="J145">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>2530</v>
       </c>
       <c r="K145">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>264.94098045273921</v>
       </c>
       <c r="M145">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>4.4675935897291854E-3</v>
       </c>
       <c r="N145">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.1836486259272232</v>
       </c>
     </row>
@@ -19486,19 +19486,19 @@
         <v>269</v>
       </c>
       <c r="J146">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>2690</v>
       </c>
       <c r="K146">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>281.69614127188476</v>
       </c>
       <c r="M146">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>4.3407023533108477E-3</v>
       </c>
       <c r="N146">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>1.2227591033374552</v>
       </c>
     </row>
@@ -19520,15 +19520,15 @@
       </c>
     </row>
     <row r="152" spans="7:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="I152" s="26" t="s">
+      <c r="I152" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J152" s="26"/>
-      <c r="K152" s="26"/>
-      <c r="L152" s="26"/>
-      <c r="M152" s="26"/>
-      <c r="N152" s="26"/>
-      <c r="O152" s="26"/>
+      <c r="J152" s="27"/>
+      <c r="K152" s="27"/>
+      <c r="L152" s="27"/>
+      <c r="M152" s="27"/>
+      <c r="N152" s="27"/>
+      <c r="O152" s="27"/>
     </row>
     <row r="154" spans="7:15" x14ac:dyDescent="0.3">
       <c r="J154" s="2" t="s">
@@ -19543,7 +19543,7 @@
         <v>0</v>
       </c>
       <c r="K155">
-        <f t="shared" ref="K155:K161" si="45">J155</f>
+        <f t="shared" ref="K155:K161" si="49">J155</f>
         <v>0</v>
       </c>
     </row>
@@ -19552,7 +19552,7 @@
         <v>325</v>
       </c>
       <c r="K156">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>325</v>
       </c>
     </row>
@@ -19561,7 +19561,7 @@
         <v>420</v>
       </c>
       <c r="K157">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>420</v>
       </c>
     </row>
@@ -19570,7 +19570,7 @@
         <v>555</v>
       </c>
       <c r="K158">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>555</v>
       </c>
     </row>
@@ -19579,7 +19579,7 @@
         <v>675</v>
       </c>
       <c r="K159">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>675</v>
       </c>
     </row>
@@ -19588,7 +19588,7 @@
         <v>805</v>
       </c>
       <c r="K160">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>805</v>
       </c>
     </row>
@@ -19597,7 +19597,7 @@
         <v>930</v>
       </c>
       <c r="K161">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>930</v>
       </c>
     </row>
@@ -19615,7 +19615,7 @@
         <v>138.5</v>
       </c>
       <c r="K163">
-        <f t="shared" ref="K163:K172" si="46">J163/0.1</f>
+        <f t="shared" ref="K163:K172" si="50">J163/0.1</f>
         <v>1385</v>
       </c>
     </row>
@@ -19624,7 +19624,7 @@
         <v>153</v>
       </c>
       <c r="K164">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>1530</v>
       </c>
     </row>
@@ -19633,7 +19633,7 @@
         <v>169</v>
       </c>
       <c r="K165">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>1690</v>
       </c>
     </row>
@@ -19642,7 +19642,7 @@
         <v>179</v>
       </c>
       <c r="K166">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>1790</v>
       </c>
     </row>
@@ -19651,7 +19651,7 @@
         <v>191</v>
       </c>
       <c r="K167">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>1910</v>
       </c>
     </row>
@@ -19660,7 +19660,7 @@
         <v>208</v>
       </c>
       <c r="K168">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2080</v>
       </c>
     </row>
@@ -19669,7 +19669,7 @@
         <v>225</v>
       </c>
       <c r="K169">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2250</v>
       </c>
     </row>
@@ -19678,7 +19678,7 @@
         <v>240</v>
       </c>
       <c r="K170">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2400</v>
       </c>
     </row>
@@ -19687,7 +19687,7 @@
         <v>253</v>
       </c>
       <c r="K171">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2530</v>
       </c>
     </row>
@@ -19696,7 +19696,7 @@
         <v>269</v>
       </c>
       <c r="K172">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2690</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated DC motor values
</commit_message>
<xml_diff>
--- a/Test Results/Motor Ra (New tests).xlsb.xlsx
+++ b/Test Results/Motor Ra (New tests).xlsb.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1776,6 +1776,411 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BG$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ke</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AZ$31:$AZ$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$BG$31:$BG$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4.3367175513452018E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0567484610800224E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8661421667244844E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7409344057481218E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.672411892432656E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6563546347673608E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6199354307522448E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5774613114320529E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5517279260957428E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5290315720430704E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5337423311972087E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5033341346503218E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4840543186105813E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4709830709454076E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4638816877558189E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.4480368037888183E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4317957598693286E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4189763321357508E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.3994873740416764E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D238-4B7B-A121-34E1AEAD03DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="410034472"/>
+        <c:axId val="410030536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="410034472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410030536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="410030536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410034472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7696,6 +8101,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8533,6 +8978,522 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13587,6 +14548,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391D7ACD-EB06-4E4B-AFEB-0452693C2DDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13887,10 +14884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:BK172"/>
+  <dimension ref="A5:CL172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BF5" sqref="BF5"/>
+    <sheetView tabSelected="1" topLeftCell="AX28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BG50" sqref="BG50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14170,7 +15167,7 @@
       <c r="AW16" s="17"/>
       <c r="AY16" s="5"/>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5.5</v>
       </c>
@@ -14190,7 +15187,7 @@
       </c>
       <c r="AW17" s="17"/>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -14210,7 +15207,7 @@
       </c>
       <c r="AW18" s="17"/>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6.5</v>
       </c>
@@ -14230,7 +15227,7 @@
       </c>
       <c r="AW19" s="17"/>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -14250,7 +15247,7 @@
       </c>
       <c r="AW20" s="17"/>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7.5</v>
       </c>
@@ -14270,7 +15267,7 @@
       </c>
       <c r="AW21" s="17"/>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>8</v>
       </c>
@@ -14290,7 +15287,7 @@
       </c>
       <c r="AW22" s="17"/>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8.5</v>
       </c>
@@ -14310,7 +15307,7 @@
       </c>
       <c r="AW23" s="17"/>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
@@ -14330,7 +15327,7 @@
       </c>
       <c r="AW24" s="17"/>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9.5</v>
       </c>
@@ -14350,7 +15347,7 @@
       </c>
       <c r="AW25" s="17"/>
     </row>
-    <row r="26" spans="1:59" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:90" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="AN26" s="27"/>
       <c r="AO26" s="27"/>
       <c r="AP26" s="27"/>
@@ -14361,10 +15358,10 @@
       <c r="AU26" s="27"/>
       <c r="AW26" s="17"/>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:90" x14ac:dyDescent="0.3">
       <c r="AW27" s="17"/>
     </row>
-    <row r="28" spans="1:59" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:90" ht="21" x14ac:dyDescent="0.4">
       <c r="K28" s="27" t="s">
         <v>10</v>
       </c>
@@ -14407,10 +15404,10 @@
       <c r="BD28" s="27"/>
       <c r="BE28" s="27"/>
     </row>
-    <row r="29" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:90" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AW29" s="17"/>
     </row>
-    <row r="30" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:90" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H30" s="29" t="s">
         <v>4</v>
       </c>
@@ -14460,7 +15457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:59" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:90" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E31" s="2" t="s">
         <v>1</v>
       </c>
@@ -14555,8 +15552,28 @@
         <f>(AZ31-$AZ$9*BA31)/BE31</f>
         <v>4.3367175513452018E-2</v>
       </c>
+      <c r="BS31" s="10"/>
+      <c r="BT31" s="10"/>
+      <c r="BU31" s="10"/>
+      <c r="BV31" s="10"/>
+      <c r="BW31" s="10"/>
+      <c r="BX31" s="10"/>
+      <c r="BY31" s="10"/>
+      <c r="BZ31" s="10"/>
+      <c r="CA31" s="10"/>
+      <c r="CB31" s="10"/>
+      <c r="CC31" s="10"/>
+      <c r="CD31" s="10"/>
+      <c r="CE31" s="10"/>
+      <c r="CF31" s="10"/>
+      <c r="CG31" s="10"/>
+      <c r="CH31" s="10"/>
+      <c r="CI31" s="10"/>
+      <c r="CJ31" s="10"/>
+      <c r="CK31" s="10"/>
+      <c r="CL31" s="10"/>
     </row>
-    <row r="32" spans="1:59" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:90" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>4.5</v>
       </c>
@@ -14660,8 +15677,9 @@
         <f t="shared" ref="BG32:BG49" si="5">(AZ32-$AZ$9*BA32)/BE32</f>
         <v>4.0567484610800224E-2</v>
       </c>
+      <c r="BS32" s="10"/>
     </row>
-    <row r="33" spans="5:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E33">
         <v>5</v>
       </c>
@@ -14763,8 +15781,9 @@
         <f t="shared" si="5"/>
         <v>3.8661421667244844E-2</v>
       </c>
+      <c r="BS33" s="10"/>
     </row>
-    <row r="34" spans="5:59" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:71" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E34">
         <v>5.5</v>
       </c>
@@ -14868,8 +15887,9 @@
         <f t="shared" si="5"/>
         <v>3.7409344057481218E-2</v>
       </c>
+      <c r="BS34" s="10"/>
     </row>
-    <row r="35" spans="5:59" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:71" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E35">
         <v>6</v>
       </c>
@@ -14973,8 +15993,9 @@
         <f t="shared" si="5"/>
         <v>3.672411892432656E-2</v>
       </c>
+      <c r="BS35" s="10"/>
     </row>
-    <row r="36" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E36">
         <v>6.5</v>
       </c>
@@ -15076,8 +16097,9 @@
         <f t="shared" si="5"/>
         <v>3.6563546347673608E-2</v>
       </c>
+      <c r="BS36" s="10"/>
     </row>
-    <row r="37" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E37">
         <v>7</v>
       </c>
@@ -15179,8 +16201,9 @@
         <f t="shared" si="5"/>
         <v>3.6199354307522448E-2</v>
       </c>
+      <c r="BS37" s="10"/>
     </row>
-    <row r="38" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E38">
         <v>7.5</v>
       </c>
@@ -15282,8 +16305,9 @@
         <f t="shared" si="5"/>
         <v>3.5774613114320529E-2</v>
       </c>
+      <c r="BS38" s="10"/>
     </row>
-    <row r="39" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E39">
         <v>8</v>
       </c>
@@ -15385,8 +16409,9 @@
         <f t="shared" si="5"/>
         <v>3.5517279260957428E-2</v>
       </c>
+      <c r="BS39" s="10"/>
     </row>
-    <row r="40" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E40">
         <v>8.5</v>
       </c>
@@ -15475,8 +16500,9 @@
         <f t="shared" si="5"/>
         <v>3.5290315720430704E-2</v>
       </c>
+      <c r="BS40" s="10"/>
     </row>
-    <row r="41" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E41">
         <v>9</v>
       </c>
@@ -15558,8 +16584,9 @@
         <f t="shared" si="5"/>
         <v>3.5337423311972087E-2</v>
       </c>
+      <c r="BS41" s="10"/>
     </row>
-    <row r="42" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E42">
         <v>9.5</v>
       </c>
@@ -15641,8 +16668,9 @@
         <f t="shared" si="5"/>
         <v>3.5033341346503218E-2</v>
       </c>
+      <c r="BS42" s="10"/>
     </row>
-    <row r="43" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E43">
         <v>10</v>
       </c>
@@ -15724,8 +16752,9 @@
         <f t="shared" si="5"/>
         <v>3.4840543186105813E-2</v>
       </c>
+      <c r="BS43" s="10"/>
     </row>
-    <row r="44" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E44">
         <v>10.5</v>
       </c>
@@ -15807,8 +16836,9 @@
         <f t="shared" si="5"/>
         <v>3.4709830709454076E-2</v>
       </c>
+      <c r="BS44" s="10"/>
     </row>
-    <row r="45" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E45">
         <v>11</v>
       </c>
@@ -15890,8 +16920,9 @@
         <f t="shared" si="5"/>
         <v>3.4638816877558189E-2</v>
       </c>
+      <c r="BS45" s="10"/>
     </row>
-    <row r="46" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E46">
         <v>11.5</v>
       </c>
@@ -15973,8 +17004,9 @@
         <f t="shared" si="5"/>
         <v>3.4480368037888183E-2</v>
       </c>
+      <c r="BS46" s="10"/>
     </row>
-    <row r="47" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E47">
         <v>12</v>
       </c>
@@ -16056,8 +17088,9 @@
         <f t="shared" si="5"/>
         <v>3.4317957598693286E-2</v>
       </c>
+      <c r="BS47" s="10"/>
     </row>
-    <row r="48" spans="5:59" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E48">
         <v>12.5</v>
       </c>
@@ -16139,8 +17172,9 @@
         <f t="shared" si="5"/>
         <v>3.4189763321357508E-2</v>
       </c>
+      <c r="BS48" s="10"/>
     </row>
-    <row r="49" spans="4:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E49">
         <v>13</v>
       </c>
@@ -16222,8 +17256,9 @@
         <f t="shared" si="5"/>
         <v>3.3994873740416764E-2</v>
       </c>
+      <c r="BS49" s="10"/>
     </row>
-    <row r="50" spans="4:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E50">
         <v>13.5</v>
       </c>
@@ -16291,7 +17326,7 @@
         <v>3.5510759501759206E-2</v>
       </c>
     </row>
-    <row r="51" spans="4:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E51">
         <v>14</v>
       </c>
@@ -16352,7 +17387,7 @@
       </c>
       <c r="AW51" s="17"/>
     </row>
-    <row r="52" spans="4:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P52" s="12">
         <f>AVERAGE(P32:P51)</f>
         <v>0.50004956219903474</v>
@@ -16373,7 +17408,7 @@
       </c>
       <c r="AW52" s="17"/>
     </row>
-    <row r="53" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:71" x14ac:dyDescent="0.3">
       <c r="J53" s="9">
         <f>4.6*2*PI()/60</f>
         <v>0.4817108735504349</v>
@@ -16384,13 +17419,13 @@
       </c>
       <c r="AW53" s="17"/>
     </row>
-    <row r="54" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:71" x14ac:dyDescent="0.3">
       <c r="AW54" s="17"/>
     </row>
-    <row r="55" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:71" x14ac:dyDescent="0.3">
       <c r="AW55" s="17"/>
     </row>
-    <row r="56" spans="4:62" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="4:71" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -16410,7 +17445,7 @@
       <c r="BF56" s="27"/>
       <c r="BG56" s="27"/>
     </row>
-    <row r="57" spans="4:62" ht="21" x14ac:dyDescent="0.4">
+    <row r="57" spans="4:71" ht="21" x14ac:dyDescent="0.4">
       <c r="H57" s="27" t="s">
         <v>36</v>
       </c>
@@ -16423,7 +17458,7 @@
       <c r="O57" s="27"/>
       <c r="AW57" s="17"/>
     </row>
-    <row r="58" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:71" x14ac:dyDescent="0.3">
       <c r="AW58" s="17"/>
       <c r="AY58" t="s">
         <v>12</v>
@@ -16456,7 +17491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:71" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>12</v>
       </c>
@@ -16512,7 +17547,7 @@
       <c r="BH59" s="4"/>
       <c r="BJ59" s="4"/>
     </row>
-    <row r="60" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:71" x14ac:dyDescent="0.3">
       <c r="E60">
         <v>40</v>
       </c>
@@ -16569,7 +17604,7 @@
       <c r="BH60" s="4"/>
       <c r="BJ60" s="4"/>
     </row>
-    <row r="61" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:71" x14ac:dyDescent="0.3">
       <c r="E61">
         <v>48</v>
       </c>
@@ -16626,7 +17661,7 @@
       <c r="BH61" s="4"/>
       <c r="BJ61" s="4"/>
     </row>
-    <row r="62" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:71" x14ac:dyDescent="0.3">
       <c r="E62">
         <v>63</v>
       </c>
@@ -16689,7 +17724,7 @@
         <v>3.304E-2</v>
       </c>
     </row>
-    <row r="63" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:71" x14ac:dyDescent="0.3">
       <c r="E63">
         <v>77</v>
       </c>
@@ -16752,7 +17787,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="64" spans="4:62" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:71" x14ac:dyDescent="0.3">
       <c r="E64">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Motor&Gears Test journal done (missing B_gears though)
</commit_message>
<xml_diff>
--- a/Test Results/Motor Ra (New tests).xlsb.xlsx
+++ b/Test Results/Motor Ra (New tests).xlsb.xlsx
@@ -14886,8 +14886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:CL172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BG50" sqref="BG50"/>
+    <sheetView tabSelected="1" topLeftCell="AY98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI102" sqref="BI102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>